<commit_message>
trying to make a waveform plot
</commit_message>
<xml_diff>
--- a/PROJECTS/MontserratML/Langer2006results.xlsx
+++ b/PROJECTS/MontserratML/Langer2006results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thompsong/src/kitchensinkGT/PROJECTS/MontserratML/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gt/src/kitchensinkGT/PROJECTS/MontserratML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CFC457-1CB0-4A4C-B9F9-E1879C1B9458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E3BB10-7F4B-2942-B9F5-563BD1F38F61}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13740" yWindow="500" windowWidth="14680" windowHeight="16360" xr2:uid="{952C77EF-CDA1-734B-818B-152200D8E967}"/>
   </bookViews>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="12">
   <si>
     <t>VTE</t>
   </si>
@@ -68,12 +59,25 @@
   <si>
     <t>accuracy</t>
   </si>
+  <si>
+    <t>precision</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -99,14 +103,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -418,15 +425,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE4739E2-4DC0-2E45-854F-A6F25CE533CF}">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>19</v>
       </c>
@@ -438,7 +445,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>5</v>
       </c>
@@ -450,7 +457,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>15</v>
       </c>
@@ -462,7 +469,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>5</v>
       </c>
@@ -474,7 +481,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>748</v>
       </c>
@@ -486,7 +493,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <f>SUM(A1:A5)</f>
         <v>792</v>
@@ -500,7 +507,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <f>A5/A6</f>
         <v>0.94444444444444442</v>
@@ -514,17 +521,17 @@
         <v>0.94736842105263153</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>0</v>
       </c>
@@ -540,8 +547,11 @@
       <c r="F11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -560,8 +570,12 @@
       <c r="F12">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="1">
+        <f>B12/SUM(B12:F12)</f>
+        <v>0.85046728971962615</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -580,8 +594,12 @@
       <c r="F13">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="1">
+        <f>C13/SUM(B13:F13)</f>
+        <v>0.72413793103448276</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -600,8 +618,12 @@
       <c r="F14">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" s="1">
+        <f>D14/SUM(B14:F14)</f>
+        <v>0.73376623376623373</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -620,8 +642,12 @@
       <c r="F15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" s="1">
+        <f>E15/SUM(B15:F15)</f>
+        <v>0.66086956521739126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -640,8 +666,12 @@
       <c r="F16">
         <v>748</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="1">
+        <f>F16/SUM(B16:F16)</f>
+        <v>0.84234234234234229</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -666,37 +696,37 @@
         <v>792</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>10</v>
       </c>
-      <c r="B18">
-        <f>B12/B17</f>
-        <v>0.80888888888888888</v>
-      </c>
-      <c r="C18">
-        <f>C13/C17</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D18">
-        <f>D14/D17</f>
-        <v>0.60427807486631013</v>
-      </c>
-      <c r="E18">
-        <f>E15/E17</f>
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="F18">
-        <f>F16/F17</f>
-        <v>0.94444444444444442</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B18" s="1">
+        <f>B23/B28</f>
+        <v>0.80911680911680917</v>
+      </c>
+      <c r="C18" s="1">
+        <f>C24/C28</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D18" s="1">
+        <f>D25/D28</f>
+        <v>0.47474747474747475</v>
+      </c>
+      <c r="E18" s="1">
+        <f>E26/E28</f>
+        <v>0.36470588235294116</v>
+      </c>
+      <c r="F18" s="1">
+        <f>F27/F28</f>
+        <v>0.95218295218295224</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>0</v>
       </c>
@@ -712,8 +742,11 @@
       <c r="F22" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -733,8 +766,12 @@
       <c r="F23">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" s="1">
+        <f>B23/SUM(B23:F23)</f>
+        <v>0.92207792207792205</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -754,8 +791,12 @@
       <c r="F24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24" s="1">
+        <f>C24/SUM(B24:F24)</f>
+        <v>0.21428571428571427</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -775,8 +816,12 @@
       <c r="F25">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25" s="1">
+        <f>D25/SUM(B25:F25)</f>
+        <v>0.61842105263157898</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -796,8 +841,12 @@
       <c r="F26">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26" s="1">
+        <f>E26/SUM(B26:F26)</f>
+        <v>0.484375</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -817,8 +866,12 @@
       <c r="F27">
         <v>458</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27" s="1">
+        <f>F27/SUM(B27:F27)</f>
+        <v>0.77627118644067794</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -843,37 +896,37 @@
         <v>481</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>10</v>
       </c>
-      <c r="B29">
-        <f>B23/B28</f>
-        <v>0.80911680911680917</v>
-      </c>
-      <c r="C29">
-        <f>C24/C28</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="D29">
-        <f>D25/D28</f>
-        <v>0.47474747474747475</v>
-      </c>
-      <c r="E29">
-        <f>E26/E28</f>
-        <v>0.36470588235294116</v>
-      </c>
-      <c r="F29">
-        <f>F27/F28</f>
-        <v>0.95218295218295224</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B29" s="1">
+        <f>B34/B39</f>
+        <v>0.80902777777777779</v>
+      </c>
+      <c r="C29" s="1">
+        <f>C35/C39</f>
+        <v>0.24242424242424243</v>
+      </c>
+      <c r="D29" s="1">
+        <f>D36/D39</f>
+        <v>0.55944055944055948</v>
+      </c>
+      <c r="E29" s="1">
+        <f>E37/E39</f>
+        <v>0.49082568807339449</v>
+      </c>
+      <c r="F29" s="1">
+        <f>F38/F39</f>
+        <v>0.94736842105263153</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>0</v>
       </c>
@@ -889,8 +942,11 @@
       <c r="F33" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -914,8 +970,12 @@
         <f t="shared" si="6"/>
         <v>28</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34" s="1">
+        <f>B34/SUM(B34:F34)</f>
+        <v>0.89272030651340994</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -939,8 +999,12 @@
         <f t="shared" si="7"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35" s="1">
+        <f>C35/SUM(B35:F35)</f>
+        <v>0.55813953488372092</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>2</v>
       </c>
@@ -964,8 +1028,12 @@
         <f t="shared" si="8"/>
         <v>23</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36" s="1">
+        <f>D36/SUM(B36:F36)</f>
+        <v>0.69565217391304346</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>3</v>
       </c>
@@ -989,8 +1057,12 @@
         <f t="shared" si="9"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37" s="1">
+        <f>E37/SUM(B37:F37)</f>
+        <v>0.5977653631284916</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -1014,8 +1086,12 @@
         <f t="shared" si="10"/>
         <v>1206</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38" s="1">
+        <f>F38/SUM(B38:F38)</f>
+        <v>0.81596752368064951</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -1040,35 +1116,29 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>10</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="1">
         <f>B34/B39</f>
         <v>0.80902777777777779</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="1">
         <f>C35/C39</f>
         <v>0.24242424242424243</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="1">
         <f>D36/D39</f>
         <v>0.55944055944055948</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="1">
         <f>E37/E39</f>
         <v>0.49082568807339449</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="1">
         <f>F38/F39</f>
         <v>0.94736842105263153</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <f>4072590/217290</f>
-        <v>18.742648074002485</v>
       </c>
     </row>
   </sheetData>

</xml_diff>